<commit_message>
Simulated Annealing documentation is done
</commit_message>
<xml_diff>
--- a/gwo_results.xlsx
+++ b/gwo_results.xlsx
@@ -15,7 +15,6 @@
     <sheet name="schwefel" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="sphere" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="zakharov" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="rotated_hyper_ellipsoid" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,10 +474,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -487,6 +486,182 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ackley</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>250</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ackley</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>250</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ackley</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>500</v>
+      </c>
+      <c r="C5" t="n">
+        <v>250</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ackley</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>500</v>
+      </c>
+      <c r="C6" t="n">
+        <v>500</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ackley</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>500</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ackley</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>250</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ackley</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>500</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ackley</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -501,7 +676,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,10 +723,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -560,6 +735,182 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>griewank</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>250</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>griewank</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>250</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>griewank</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>500</v>
+      </c>
+      <c r="C5" t="n">
+        <v>250</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>griewank</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>500</v>
+      </c>
+      <c r="C6" t="n">
+        <v>500</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>griewank</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>500</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>griewank</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>250</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>griewank</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>500</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>griewank</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -574,7 +925,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,10 +972,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -633,6 +984,182 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>perm</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>250</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>perm</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>250</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>perm</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>500</v>
+      </c>
+      <c r="C5" t="n">
+        <v>250</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>perm</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>500</v>
+      </c>
+      <c r="C6" t="n">
+        <v>500</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>perm</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>500</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>perm</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>250</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>perm</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>500</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>perm</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -647,7 +1174,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -694,10 +1221,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -706,6 +1233,182 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>rastrigin</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>250</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>rastrigin</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>250</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>rastrigin</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>500</v>
+      </c>
+      <c r="C5" t="n">
+        <v>250</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>rastrigin</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>500</v>
+      </c>
+      <c r="C6" t="n">
+        <v>500</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rastrigin</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>500</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>rastrigin</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>250</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>rastrigin</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>500</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>rastrigin</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -720,7 +1423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,10 +1470,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -779,6 +1482,182 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>rosenbrock</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>250</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>rosenbrock</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>250</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>rosenbrock</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>500</v>
+      </c>
+      <c r="C5" t="n">
+        <v>250</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>rosenbrock</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>500</v>
+      </c>
+      <c r="C6" t="n">
+        <v>500</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rosenbrock</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>500</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>rosenbrock</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>250</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>rosenbrock</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>500</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>rosenbrock</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -793,7 +1672,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -840,10 +1719,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -852,6 +1731,182 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>schwefel</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>250</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>schwefel</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>250</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>schwefel</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>500</v>
+      </c>
+      <c r="C5" t="n">
+        <v>250</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>schwefel</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>500</v>
+      </c>
+      <c r="C6" t="n">
+        <v>500</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>schwefel</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>500</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>schwefel</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>250</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>schwefel</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>500</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>schwefel</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -866,7 +1921,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -913,10 +1968,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -925,6 +1980,182 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sphere</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>250</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sphere</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>250</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sphere</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>500</v>
+      </c>
+      <c r="C5" t="n">
+        <v>250</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sphere</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>500</v>
+      </c>
+      <c r="C6" t="n">
+        <v>500</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sphere</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>500</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sphere</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>250</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sphere</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>500</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>sphere</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -939,7 +2170,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -986,91 +2217,194 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Function</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Population Size</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Number of Generations</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Best Fitness</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Best Average Fitness</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Std_Dev Fitness</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>rotated_hyper_ellipsoid</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>100</v>
-      </c>
-      <c r="C2" t="n">
-        <v>100</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>zakharov</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>250</v>
+      </c>
+      <c r="C3" t="n">
+        <v>500</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>zakharov</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>250</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>zakharov</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>500</v>
+      </c>
+      <c r="C5" t="n">
+        <v>250</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>zakharov</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>500</v>
+      </c>
+      <c r="C6" t="n">
+        <v>500</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>zakharov</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>500</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>zakharov</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>250</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>zakharov</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>500</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>zakharov</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>